<commit_message>
Thu Jan 30 06:29:49 PM EST 2025 SHAP curves
</commit_message>
<xml_diff>
--- a/iron_oxo_DDCASPT2/iron_VDZP_SHAP.xlsx
+++ b/iron_oxo_DDCASPT2/iron_VDZP_SHAP.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C106"/>
+  <dimension ref="A1:C103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -447,189 +447,189 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>26</v>
+        <v>63</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>typ_3</t>
+          <t>$(\eta_{p})_{3}$</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.0003030520996821289</v>
+        <v>0.0004157567213702839</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>$F_{q}^{\text{SCF}}$</t>
+          <t>h$_{q}$</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.0002265110449524768</v>
+        <v>0.000290139374458511</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>74</v>
+        <v>34</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>$\langle qq \vert qq \rangle$</t>
+          <t>$F_{q}$</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.0001802233439045941</v>
+        <v>0.0002273424484478815</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>12</v>
+        <v>71</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>h$_{q}$</t>
+          <t>$\langle qq \vert qq \rangle$</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.0001654739209145547</v>
+        <v>0.0001623723393554985</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>$\omega_{q}$</t>
+          <t>type_0</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.0001142489385971482</v>
+        <v>0.0001334928622807003</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>$F_{q}$</t>
+          <t>$\eta_{q}$</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.000113023469022269</v>
+        <v>0.0001239896895613397</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>76</v>
+        <v>25</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>$\langle ss \vert ss \rangle$</t>
+          <t>type_2</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>9.976776534242466e-05</v>
+        <v>0.0001161569630488966</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>$\omega_{s}$</t>
+          <t>h$_{s}$</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>9.967559229596801e-05</v>
+        <v>0.000110561736628257</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>$(\omega_{p})_{3}$</t>
+          <t>$(\eta_{r})_{1}$</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>9.059775466200577e-05</v>
+        <v>0.0001096504657186124</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>typ_2</t>
+          <t>$\omega_{q}$</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>8.580763848886006e-05</v>
+        <v>7.629534489682738e-05</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>22</v>
+        <v>82</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>h$_{s}$</t>
+          <t>$(\langle pq \vert pq \rangle)_{1}$</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>7.749482587529105e-05</v>
+        <v>7.046730410026125e-05</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>$(\eta_{p})_{3}$</t>
+          <t>$(\omega_{r})_{2}$</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>7.430892066882528e-05</v>
+        <v>5.517289093263244e-05</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>68</v>
+        <v>97</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>$(\omega_{r})_{3}$</t>
+          <t>$(\langle rr \vert rr \rangle)_{3}$</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>6.810108483093589e-05</v>
+        <v>5.507872675448896e-05</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>$F_{s}$</t>
+          <t>$F_{s}^{\text{SCF}}$</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>6.55865712563689e-05</v>
+        <v>5.309151161450792e-05</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -637,675 +637,675 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>5.590554966209538e-05</v>
+        <v>5.10778340103672e-05</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>$\eta_{q}$</t>
+          <t>$\omega_{s}$</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>5.140981874380032e-05</v>
+        <v>5.044993804635663e-05</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>79</v>
+        <v>56</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>$(\langle rs\vert rs \rangle)_{0}$</t>
+          <t>$(F_{r}^{\text{SCF}})_{2}$</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>4.090201130477832e-05</v>
+        <v>5.010402019395764e-05</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>102</v>
+        <v>37</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert qp \rangle)_{3}$</t>
+          <t>$(\omega_{r})_{0}$</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>3.956526426174663e-05</v>
+        <v>4.960331058271254e-05</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>43</v>
+        <v>64</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>$F_{s}^{\text{SCF}}$</t>
+          <t>$(F_{r}^{\text{SCF}})_{3}$</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>3.78182580225615e-05</v>
+        <v>4.772730274940301e-05</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>FA$_{qs}$</t>
+          <t>$(\omega_{r})_{1}$</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>3.770594382706313e-05</v>
+        <v>4.600838046536132e-05</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>typ_1</t>
+          <t>$(\omega_{p})_{2}$</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>3.605465595535284e-05</v>
+        <v>4.564606277106112e-05</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>86</v>
+        <v>32</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert qp \rangle)_{1}$</t>
+          <t>$F_{q}^{\text{SCF}}$</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>3.395363495651337e-05</v>
+        <v>4.370306702270499e-05</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>$(F_{r})_{0}$</t>
+          <t>h$_{qs}$</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>3.246707516612103e-05</v>
+        <v>4.241313879659445e-05</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>104</v>
+        <v>73</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>$(\langle rs \vert sr \rangle)_{3}$</t>
+          <t>$\langle ss \vert ss \rangle$</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>3.161987633730667e-05</v>
+        <v>3.955004882625746e-05</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>$(\langle rr \vert rr \rangle)_{3}$</t>
+          <t>$(\langle pp \vert pp \rangle)_{3}$</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>3.097017555094772e-05</v>
+        <v>3.761537300470821e-05</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>65</v>
+        <v>0</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>$(F_{p})_{3}$</t>
+          <t>(h$_{p}$)$_{0}$</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>3.021484893565001e-05</v>
+        <v>3.539829919078683e-05</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>78</v>
+        <v>42</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert qp \rangle)_{0}$</t>
+          <t>$F_{s}$</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>2.831158342919164e-05</v>
+        <v>3.419683270335941e-05</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>101</v>
+        <v>26</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert pq \rangle)_{3}$</t>
+          <t>type_3</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>2.783727836048292e-05</v>
+        <v>3.386560109890882e-05</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>103</v>
+        <v>16</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>$(\langle rs\vert rs \rangle)_{3}$</t>
+          <t>(h$_{r}$)$_{2}$</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>2.774734976962165e-05</v>
+        <v>3.257593287023475e-05</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>60</v>
+        <v>99</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>$(\omega_{r})_{2}$</t>
+          <t>$(\langle pq \vert qp \rangle)_{3}$</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>2.714586139958707e-05</v>
+        <v>3.13977160646603e-05</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>69</v>
+        <v>90</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>$(F_{r})_{3}$</t>
+          <t>$(\langle pq \vert pq \rangle)_{2}$</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>2.683895949570908e-05</v>
+        <v>3.067891986185492e-05</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>$(\langle pp \vert pp \rangle)_{0}$</t>
+          <t>$(\langle pq \vert rs \rangle)_{1}$</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>2.621204238687618e-05</v>
+        <v>2.980397308013429e-05</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>29</v>
+        <v>98</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>FI$_{qs}$</t>
+          <t>$(\langle pq \vert pq \rangle)_{3}$</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>2.521112668702972e-05</v>
+        <v>2.925659744673746e-05</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>h$_{qs}$</t>
+          <t>$(F_{p})_{1}$</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>2.517173349425311e-05</v>
+        <v>2.901542041992879e-05</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>96</v>
+        <v>52</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>$(\langle rs \vert sr \rangle)_{2}$</t>
+          <t>$(F_{p}^{\text{SCF}})_{2}$</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>2.248696042768056e-05</v>
+        <v>2.89305407774203e-05</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>16</v>
+        <v>65</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>h$_{r}^{2}$</t>
+          <t>$(\omega_{r})_{3}$</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>2.125917547041695e-05</v>
+        <v>2.77700738545241e-05</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>h$_{pq}^{3}$</t>
+          <t>(h$_{r}$)$_{3}$</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>2.047295345509963e-05</v>
+        <v>2.752337336755773e-05</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
-        <v>94</v>
+        <v>70</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert qp \rangle)_{2}$</t>
+          <t>$(\langle pp \vert pp \rangle)_{0}$</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>2.040069721603855e-05</v>
+        <v>2.572705361130168e-05</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
-        <v>3</v>
+        <v>62</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>h$_{p}^{3}$</t>
+          <t>$(F_{p})_{3}$</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>1.985845160629837e-05</v>
+        <v>2.498604767370821e-05</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>$(\omega_{p})_{1}$</t>
+          <t>$(\eta_{r})_{2}$</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>1.908666811772434e-05</v>
+        <v>2.459154450062279e-05</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
-        <v>85</v>
+        <v>3</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert pq \rangle)_{1}$</t>
+          <t>(h$_{p}$)$_{3}$</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>1.833271739213631e-05</v>
+        <v>2.383854342962097e-05</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
-        <v>23</v>
+        <v>89</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>typ_0</t>
+          <t>$(\langle rr \vert rr \rangle)_{2}$</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>1.831390708624104e-05</v>
+        <v>2.247724622789276e-05</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>$(F_{r})_{1}$</t>
+          <t>$(\eta_{r})_{3}$</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>1.825721419601705e-05</v>
+        <v>2.201944833349865e-05</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
-        <v>52</v>
+        <v>101</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>$(\omega_{r})_{1}$</t>
+          <t>$(\langle rs \vert sr \rangle)_{3}$</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>1.805827799975887e-05</v>
+        <v>2.19368952904614e-05</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
-        <v>99</v>
+        <v>2</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>$(\langle pp \vert pp \rangle)_{3}$</t>
+          <t>(h$_{p}$)$_{2}$</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>1.734044556937801e-05</v>
+        <v>2.184268460733789e-05</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
-        <v>89</v>
+        <v>44</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert rs \rangle)_{2}$</t>
+          <t>$(F_{p}^{\text{SCF}})_{1}$</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>1.729625226315301e-05</v>
+        <v>2.149826559738942e-05</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
-        <v>95</v>
+        <v>66</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>$(\langle rs\vert rs \rangle)_{2}$</t>
+          <t>$(F_{r})_{3}$</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>1.726397600615352e-05</v>
+        <v>2.137882349879637e-05</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
-        <v>6</v>
+        <v>74</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>h$_{pq}^{2}$</t>
+          <t>$(\langle pq \vert pq \rangle)_{0}$</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>1.597368532320217e-05</v>
+        <v>2.088678196915421e-05</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
-        <v>88</v>
+        <v>1</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>$(\langle rs \vert sr \rangle)_{1}$</t>
+          <t>(h$_{p}$)$_{1}$</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>1.552910288251795e-05</v>
+        <v>2.081343384979578e-05</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>h$_{p}^{1}$</t>
+          <t>$(F_{p}^{\text{SCF}})_{0}$</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>1.528678294011606e-05</v>
+        <v>2.057832566375867e-05</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>$(F_{p})_{2}$</t>
+          <t>$(\omega_{p})_{3}$</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>1.516549336587947e-05</v>
+        <v>2.007224768621259e-05</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
-        <v>97</v>
+        <v>24</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert rs \rangle)_{3}$</t>
+          <t>type_1</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>1.500081348092622e-05</v>
+        <v>1.882612331334603e-05</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>h$_{p}^{0}$</t>
+          <t>$(\langle pq \vert qp \rangle)_{0}$</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>1.492164454913991e-05</v>
+        <v>1.833907879362257e-05</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>$(\eta_{p})_{1}$</t>
+          <t>$(F_{r}^{\text{SCF}})_{1}$</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>1.482846160858861e-05</v>
+        <v>1.833640742032477e-05</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
-        <v>59</v>
+        <v>85</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>$(F_{r}^{\text{SCF}})_{2}$</t>
+          <t>$(\langle rs \vert sr \rangle)_{1}$</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>1.45001949138058e-05</v>
+        <v>1.756112624606058e-05</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>h$_{pr}^{1}$</t>
+          <t>(h$_{rs}$)$_{3}$</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>1.424912923073026e-05</v>
+        <v>1.697722173460098e-05</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
-        <v>83</v>
+        <v>45</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>$(\langle pp \vert pp \rangle)_{1}$</t>
+          <t>$(\omega_{p})_{1}$</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>1.424382368406034e-05</v>
+        <v>1.615137454610847e-05</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
-        <v>15</v>
+        <v>93</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>h$_{r}^{1}$</t>
+          <t>$(\langle rs \vert sr \rangle)_{2}$</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>1.419653187356243e-05</v>
+        <v>1.42425486691933e-05</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>h$_{rs}^{3}$</t>
+          <t>(h$_{r}$)$_{1}$</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>1.403729019372445e-05</v>
+        <v>1.417339657005311e-05</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>h$_{r}^{3}$</t>
+          <t>$(F_{r})_{2}$</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>1.361025958522298e-05</v>
+        <v>1.414233453407028e-05</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert pq \rangle)_{2}$</t>
+          <t>$(\langle rs\vert rs \rangle)_{2}$</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>1.315869780312337e-05</v>
+        <v>1.389693782803359e-05</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
-        <v>14</v>
+        <v>54</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>h$_{r}^{0}$</t>
+          <t>$(F_{p})_{2}$</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>1.293212687384211e-05</v>
+        <v>1.381934279343663e-05</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
-        <v>2</v>
+        <v>100</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>h$_{p}^{2}$</t>
+          <t>$(\langle rs\vert rs \rangle)_{3}$</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>1.292119864943596e-05</v>
+        <v>1.370711653207472e-05</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
-        <v>77</v>
+        <v>55</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert pq \rangle)_{0}$</t>
+          <t>$(\eta_{p})_{2}$</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>1.278277224008261e-05</v>
+        <v>1.356167335057485e-05</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>$(F_{r}^{\text{SCF}})_{3}$</t>
+          <t>$(\eta_{p})_{1}$</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>1.268029594526181e-05</v>
+        <v>1.353140015090087e-05</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
-        <v>19</v>
+        <v>83</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>h$_{rs}^{1}$</t>
+          <t>$(\langle pq \vert qp \rangle)_{1}$</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>1.217530619135382e-05</v>
+        <v>1.340289720978328e-05</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
@@ -1313,389 +1313,389 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>1.197467490789259e-05</v>
+        <v>1.295423290746717e-05</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>$(F_{r})_{2}$</t>
+          <t>$(\omega_{p})_{0}$</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>1.193782040140949e-05</v>
+        <v>1.24408246171908e-05</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>$(\langle rr \vert rr \rangle)_{2}$</t>
+          <t>$(\langle pq \vert qp \rangle)_{2}$</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>1.179571734000235e-05</v>
+        <v>1.225725256572459e-05</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
-        <v>32</v>
+        <v>81</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>$(\omega_{p})_{0}$</t>
+          <t>$(\langle rr \vert rr \rangle)_{1}$</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>1.159455177385357e-05</v>
+        <v>1.197613117076442e-05</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>$(F_{p})_{1}$</t>
+          <t>$(F_{p}^{\text{SCF}})_{3}$</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>1.15764448281507e-05</v>
+        <v>1.159350821073504e-05</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
-        <v>39</v>
+        <v>72</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>$(F_{r}^{\text{SCF}})_{0}$</t>
+          <t>$(\langle rr \vert rr \rangle)_{0}$</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>1.156096976417175e-05</v>
+        <v>1.042288120106709e-05</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
-        <v>70</v>
+        <v>88</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>$(\eta_{r})_{3}$</t>
+          <t>$(\langle pp \vert pp \rangle)_{2}$</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>1.153515003449703e-05</v>
+        <v>1.038051783149002e-05</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
-        <v>56</v>
+        <v>7</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>$(\omega_{p})_{2}$</t>
+          <t>(h$_{pq}$)$_{3}$</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>1.111302259211201e-05</v>
+        <v>9.634887593523372e-06</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
-        <v>91</v>
+        <v>50</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>$(\langle pp \vert pp \rangle)_{2}$</t>
+          <t>$(F_{r})_{1}$</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>1.100231691942118e-05</v>
+        <v>9.557339853405346e-06</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>h$_{pr}^{2}$</t>
+          <t>$(F_{p})_{0}$</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>1.076243079873221e-05</v>
+        <v>9.486032456692025e-06</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
-        <v>63</v>
+        <v>5</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>$(F_{p}^{\text{SCF}})_{3}$</t>
+          <t>(h$_{pq}$)$_{1}$</t>
         </is>
       </c>
       <c r="C78" t="n">
-        <v>9.83319772290225e-06</v>
+        <v>8.998809634732034e-06</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>$(\langle rr \vert rr \rangle)_{1}$</t>
+          <t>$(\langle rs \vert sr \rangle)_{0}$</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>9.825834109785978e-06</v>
+        <v>8.833259652867683e-06</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>h$_{pr}^{3}$</t>
+          <t>$(F_{r}^{\text{SCF}})_{0}$</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>9.743545669315042e-06</v>
+        <v>8.776570897784947e-06</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
-        <v>80</v>
+        <v>6</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>$(\langle rs \vert sr \rangle)_{0}$</t>
+          <t>(h$_{pq}$)$_{2}$</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>9.359702517575303e-06</v>
+        <v>8.637085836809696e-06</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>h$_{rs}^{2}$</t>
+          <t>$(\langle rs\vert rs \rangle)_{0}$</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>8.538651122976053e-06</v>
+        <v>8.53892463609517e-06</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>h$_{rs}^{0}$</t>
+          <t>$(\eta_{r})_{0}$</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>8.322325221442837e-06</v>
+        <v>7.593694353310427e-06</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>$(\eta_{r})_{2}$</t>
+          <t>$(\langle pp \vert pp \rangle)_{1}$</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>7.643201647984068e-06</v>
+        <v>7.561366840267867e-06</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>$(F_{p})_{0}$</t>
+          <t>(h$_{rs}$)$_{2}$</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>7.630533811390378e-06</v>
+        <v>6.692610970674523e-06</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
-        <v>47</v>
+        <v>19</v>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>$(F_{p}^{\text{SCF}})_{1}$</t>
+          <t>(h$_{rs}$)$_{1}$</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>7.468530304169827e-06</v>
+        <v>6.482236256891163e-06</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>$(\eta_{r})_{1}$</t>
+          <t>(h$_{pr}$)$_{2}$</t>
         </is>
       </c>
       <c r="C87" t="n">
-        <v>6.447570963215746e-06</v>
+        <v>6.140238784831359e-06</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
-        <v>58</v>
+        <v>8</v>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>$(\eta_{p})_{2}$</t>
+          <t>(h$_{pr}$)$_{0}$</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>5.482298626656158e-06</v>
+        <v>5.305549477198354e-06</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>$(\omega_{r})_{0}$</t>
+          <t>(h$_{r}$)$_{0}$</t>
         </is>
       </c>
       <c r="C89" t="n">
-        <v>5.289885088870167e-06</v>
+        <v>5.188536036689117e-06</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>h$_{pq}^{1}$</t>
+          <t>(h$_{rs}$)$_{0}$</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>5.212971964847599e-06</v>
+        <v>4.882071955346145e-06</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>$(F_{p}^{\text{SCF}})_{0}$</t>
+          <t>(h$_{pr}$)$_{1}$</t>
         </is>
       </c>
       <c r="C91" t="n">
-        <v>5.126293750181973e-06</v>
+        <v>4.631316378079669e-06</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
-        <v>4</v>
+        <v>86</v>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>h$_{pq}^{0}$</t>
+          <t>$(\langle pq \vert rs \rangle)_{2}$</t>
         </is>
       </c>
       <c r="C92" t="n">
-        <v>4.732255835533819e-06</v>
+        <v>4.53979300601717e-06</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
-        <v>75</v>
+        <v>4</v>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>$(\langle rr \vert rr \rangle)_{0}$</t>
+          <t>(h$_{pq}$)$_{0}$</t>
         </is>
       </c>
       <c r="C93" t="n">
-        <v>4.713135611734086e-06</v>
+        <v>4.415802633096471e-06</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
-        <v>51</v>
+        <v>94</v>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>$(F_{r}^{\text{SCF}})_{1}$</t>
+          <t>$(\langle pq \vert rs \rangle)_{3}$</t>
         </is>
       </c>
       <c r="C94" t="n">
-        <v>4.542534448211638e-06</v>
+        <v>4.058401268581065e-06</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
-        <v>55</v>
+        <v>11</v>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>$(F_{p}^{\text{SCF}})_{2}$</t>
+          <t>(h$_{pr}$)$_{3}$</t>
         </is>
       </c>
       <c r="C95" t="n">
-        <v>4.34931671820895e-06</v>
+        <v>3.296270583498369e-06</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>h$_{pr}^{0}$</t>
+          <t>$(F_{r})_{0}$</t>
         </is>
       </c>
       <c r="C96" t="n">
-        <v>3.575304303113552e-06</v>
+        <v>2.728685194101913e-06</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert rs \rangle)_{1}$</t>
+          <t>$(\langle pq \vert rs \rangle)_{0}$</t>
         </is>
       </c>
       <c r="C97" t="n">
-        <v>3.32917539426503e-06</v>
+        <v>1.618991886867202e-06</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="n">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B98" t="inlineStr">
         <is>
@@ -1703,111 +1703,72 @@
         </is>
       </c>
       <c r="C98" t="n">
-        <v>3.251166475105681e-06</v>
+        <v>1.498307331997344e-06</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="n">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert rs \rangle)_{0}$</t>
+          <t>$(\langle pq \vert sr \rangle)_{2}$</t>
         </is>
       </c>
       <c r="C99" t="n">
-        <v>3.229273683855082e-06</v>
+        <v>2.200929839259728e-07</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
-        <v>42</v>
+        <v>69</v>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>$(\eta_{r})_{0}$</t>
+          <t>$(\langle pq \vert sr \rangle)_{0}$</t>
         </is>
       </c>
       <c r="C100" t="n">
-        <v>1.801626703913815e-06</v>
+        <v>2.027501266921313e-07</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert sr \rangle)_{2}$</t>
+          <t>$(\langle pq \vert sr \rangle)_{1}$</t>
         </is>
       </c>
       <c r="C101" t="n">
-        <v>4.281090786922626e-07</v>
+        <v>1.904500267532901e-07</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="1" t="n">
-        <v>72</v>
+        <v>95</v>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert sr \rangle)_{0}$</t>
+          <t>$(\langle pq \vert sr \rangle)_{3}$</t>
         </is>
       </c>
       <c r="C102" t="n">
-        <v>4.229080142829116e-07</v>
+        <v>1.803912406261183e-07</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="1" t="n">
-        <v>98</v>
+        <v>27</v>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert sr \rangle)_{3}$</t>
+          <t>$\mathbf{b}$</t>
         </is>
       </c>
       <c r="C103" t="n">
-        <v>4.174754933731055e-07</v>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" s="1" t="n">
-        <v>82</v>
-      </c>
-      <c r="B104" t="inlineStr">
-        <is>
-          <t>$(\langle pq \vert sr \rangle)_{1}$</t>
-        </is>
-      </c>
-      <c r="C104" t="n">
-        <v>4.052606050283023e-07</v>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" s="1" t="n">
-        <v>28</v>
-      </c>
-      <c r="B105" t="inlineStr">
-        <is>
-          <t>F$_{qs}$</t>
-        </is>
-      </c>
-      <c r="C105" t="n">
-        <v>3.465864559314345e-07</v>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" s="1" t="n">
-        <v>27</v>
-      </c>
-      <c r="B106" t="inlineStr">
-        <is>
-          <t>$\mathbf{b}$</t>
-        </is>
-      </c>
-      <c r="C106" t="n">
-        <v>3.914808141833531e-08</v>
+        <v>2.214120663739143e-08</v>
       </c>
     </row>
   </sheetData>

</xml_diff>